<commit_message>
Updated the achievements spreadsheet
</commit_message>
<xml_diff>
--- a/achievements.xlsx
+++ b/achievements.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Achivment</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Get Power Up #3 100 times</t>
+  </si>
+  <si>
+    <t>Get Power Up #4 10 times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Power Up #4 50 times </t>
+  </si>
+  <si>
+    <t>Get Power Up #4 100 times</t>
   </si>
 </sst>
 </file>
@@ -171,8 +180,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -184,13 +197,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -524,7 +541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -633,90 +650,168 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>31</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -725,7 +820,7 @@
       </c>
       <c r="B40">
         <f>SUM(B2:B39)</f>
-        <v>210</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes to achievements doc
</commit_message>
<xml_diff>
--- a/achievements.xlsx
+++ b/achievements.xlsx
@@ -347,10 +347,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -712,13 +715,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="48" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" customWidth="1"/>
     <col min="3" max="3" width="53.33203125" customWidth="1"/>
     <col min="4" max="4" width="32.1640625" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
@@ -1208,7 +1211,7 @@
       <c r="A33">
         <v>20</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>365</v>
       </c>
       <c r="C33" t="s">

</xml_diff>